<commit_message>
Write test status in Excel first try
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
-    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
+    <sheet sheetId="3" r:id="rId3" name="DataSetInteractionPages"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataSetInteractionPages!$A$1:$A$27</definedName>
+    <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="122">
   <si>
     <t>Key</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>AssertHomePageLogoDisplayed</t>
+  </si>
+  <si>
+    <t>passed</t>
   </si>
 </sst>
 </file>
@@ -946,14 +949,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.90625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -972,7 +975,7 @@
     <col min="15" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
         <v>93</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="2">
       <c r="A2" s="6" t="s">
         <v>95</v>
       </c>
@@ -1057,7 +1060,7 @@
       </c>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
@@ -1091,7 +1094,7 @@
       </c>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="5">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6">
@@ -1165,7 +1168,7 @@
       </c>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="6">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -1199,7 +1202,7 @@
       </c>
       <c r="N6" s="6"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="7">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6">
@@ -1233,7 +1236,7 @@
       </c>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="8">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6">
@@ -1267,7 +1270,7 @@
       </c>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="9">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -1301,7 +1304,7 @@
       </c>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="10">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -1335,7 +1338,7 @@
       </c>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="11">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -1367,7 +1370,7 @@
       </c>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="12">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6">
@@ -1401,7 +1404,7 @@
       </c>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="13">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -1435,7 +1438,7 @@
       </c>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="14">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -1469,7 +1472,7 @@
       </c>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="15">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6">
@@ -1503,7 +1506,7 @@
       </c>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="16">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6">
@@ -1537,7 +1540,7 @@
       </c>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="17">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -1569,7 +1572,7 @@
       </c>
       <c r="N17" s="6"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="18">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -1603,7 +1606,7 @@
       </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="19">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6">
@@ -1635,7 +1638,7 @@
       </c>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="20">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6">
@@ -1669,7 +1672,7 @@
       </c>
       <c r="N20" s="6"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="21">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6">
@@ -1703,7 +1706,7 @@
       </c>
       <c r="N21" s="6"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
         <v>111</v>
       </c>
@@ -1736,8 +1739,13 @@
       <c r="N22" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O22" s="2" t="inlineStr">
+        <is>
+          <t>New Name</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:15" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1746,7 +1754,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1755,7 +1763,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>

</xml_diff>

<commit_message>
Write test status in Excel
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -58,7 +58,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>vankatabe:</t>
         </r>
@@ -67,7 +68,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Expected Effect - displayed error message, displayed rows, etc.</t>
@@ -92,7 +94,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>vankatabe:</t>
         </r>
@@ -101,7 +104,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 size constraint</t>
@@ -116,7 +120,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">vankatabe:
 </t>
@@ -488,29 +493,29 @@
     <t>blog's address</t>
   </si>
   <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Asserter</t>
+  </si>
+  <si>
+    <t>CheckWebSiteLoad_EnterBlogURL_OpenBlogHomePage</t>
+  </si>
+  <si>
+    <t>AssertHomePageLogoDisplayed</t>
+  </si>
+  <si>
     <t>SOFTUNI BLOG</t>
   </si>
   <si>
-    <t>Effect</t>
-  </si>
-  <si>
-    <t>Asserter</t>
-  </si>
-  <si>
-    <t>CheckWebSiteLoad_EnterBlogURL_OpenBlogHomePage</t>
-  </si>
-  <si>
-    <t>AssertHomePageLogoDisplayed</t>
-  </si>
-  <si>
-    <t>passed</t>
+    <t>prona</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,19 +546,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -608,12 +600,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -953,7 +960,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1013,10 +1020,10 @@
         <v>7</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>108</v>
@@ -1727,21 +1734,21 @@
         <v>115</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O22" s="2" t="inlineStr">
         <is>
-          <t>New Name</t>
+          <t>passed</t>
         </is>
       </c>
     </row>
@@ -1773,6 +1780,14 @@
       <c r="G25" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="failed">
+      <formula>NOT(ISERROR(SEARCH("failed",O1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Add first RegisterPage test, Add unique User ID
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
-    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
-    <sheet sheetId="3" r:id="rId3" name="DataSetInteractionPages"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
+    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -73,6 +73,32 @@
           </rPr>
           <t xml:space="preserve">
 Expected Effect - displayed error message, displayed rows, etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>vankatabe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+The test framework automatically fills-in the result!</t>
         </r>
       </text>
     </comment>
@@ -143,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="126">
   <si>
     <t>Key</t>
   </si>
@@ -223,9 +249,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>First name</t>
-  </si>
-  <si>
     <t>missing</t>
   </si>
   <si>
@@ -457,24 +480,15 @@
     <t>Test Case ID</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
     <t>valid</t>
   </si>
   <si>
-    <t>FullName</t>
-  </si>
-  <si>
     <t>Register_UniqueCredentials_RegisterSuccessful</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>passed / failed</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -487,12 +501,6 @@
     <t>9.1</t>
   </si>
   <si>
-    <t>browser go-to address</t>
-  </si>
-  <si>
-    <t>blog's address</t>
-  </si>
-  <si>
     <t>Effect</t>
   </si>
   <si>
@@ -508,7 +516,37 @@
     <t>SOFTUNI BLOG</t>
   </si>
   <si>
-    <t>prona</t>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>valid Blog web address</t>
+  </si>
+  <si>
+    <t>register form - all</t>
+  </si>
+  <si>
+    <t>browser go-to - address</t>
+  </si>
+  <si>
+    <t>AssertGreetingDisplayed</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Fullname</t>
+  </si>
+  <si>
+    <t>&lt;Fullname@uniqueemail.com&gt;</t>
+  </si>
+  <si>
+    <t>&lt;unique generated per test suite&gt;</t>
+  </si>
+  <si>
+    <t>article list</t>
+  </si>
+  <si>
+    <t>at least one article exists</t>
   </si>
 </sst>
 </file>
@@ -588,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -601,11 +639,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -956,14 +1004,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -974,7 +1022,7 @@
     <col min="7" max="7" width="16.1796875" style="2" customWidth="1"/>
     <col min="8" max="8" width="46.26953125" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.26953125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.26953125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.36328125" style="2" customWidth="1"/>
     <col min="11" max="11" width="9.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.7265625" style="2" customWidth="1"/>
@@ -982,27 +1030,27 @@
     <col min="15" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:15" outlineLevel="0" r="1">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1011,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -1020,32 +1068,32 @@
         <v>7</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
@@ -1062,24 +1110,24 @@
       <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="M2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>11</v>
@@ -1096,39 +1144,41 @@
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="4">
+      <c r="M3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="F4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>8</v>
+      <c r="I4" t="s">
+        <v>122</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>10</v>
@@ -1136,24 +1186,29 @@
       <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6">
+      <c r="M4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>12</v>
@@ -1170,24 +1225,24 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="6">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6">
+      <c r="M5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>27</v>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
@@ -1204,24 +1259,24 @@
       <c r="L6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N6" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6">
+      <c r="M6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>14</v>
@@ -1238,24 +1293,24 @@
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6">
+      <c r="M7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4">
         <v>7</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>33</v>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>15</v>
@@ -1272,24 +1327,24 @@
       <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N8" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6">
+      <c r="M8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4">
         <v>8</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>27</v>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>16</v>
@@ -1306,24 +1361,24 @@
       <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N9" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6">
+      <c r="M9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4">
         <v>9</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>34</v>
+      <c r="G10" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>17</v>
@@ -1340,24 +1395,24 @@
       <c r="L10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6" t="s">
+      <c r="M10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>27</v>
+      <c r="G11" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>18</v>
@@ -1372,24 +1427,24 @@
       <c r="L11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N11" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="12">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6">
+      <c r="M11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4">
         <v>11</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>35</v>
+      <c r="G12" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>19</v>
@@ -1406,24 +1461,24 @@
       <c r="L12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="13">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6">
+      <c r="M12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4">
         <v>12</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>36</v>
+      <c r="G13" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>21</v>
@@ -1440,24 +1495,24 @@
       <c r="L13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N13" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="14">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6">
+      <c r="M13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4">
         <v>13</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>37</v>
+      <c r="G14" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>23</v>
@@ -1474,27 +1529,27 @@
       <c r="L14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="N14" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6">
+      <c r="M14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4">
         <v>14</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>34</v>
+      <c r="G15" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>8</v>
@@ -1508,61 +1563,61 @@
       <c r="L15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N15" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="16">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6">
+      <c r="M15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4">
         <v>15</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="17">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6">
-        <v>17</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>8</v>
@@ -1574,27 +1629,27 @@
       <c r="L17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N17" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="18">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6">
+      <c r="M17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4">
         <v>18</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>32</v>
+      <c r="G18" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>8</v>
@@ -1603,32 +1658,32 @@
         <v>9</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N18" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="19">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6">
+      <c r="M18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4">
         <v>19</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>27</v>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>8</v>
@@ -1640,27 +1695,27 @@
         <v>10</v>
       </c>
       <c r="L19" s="3"/>
-      <c r="M19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N19" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="20">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6">
+      <c r="M19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4">
         <v>20</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>8</v>
@@ -1672,29 +1727,29 @@
         <v>10</v>
       </c>
       <c r="L20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4">
+        <v>21</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N20" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="21">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6">
-        <v>21</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>8</v>
@@ -1706,53 +1761,53 @@
         <v>10</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N21" s="6"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="22">
+        <v>61</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="6" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="O22" s="2" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="23">
+        <v>113</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1761,7 +1816,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row spans="1:15" outlineLevel="0" r="24">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1770,7 +1825,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row spans="1:15" outlineLevel="0" r="25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1781,11 +1836,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="failed">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="failed">
       <formula>NOT(ISERROR(SEARCH("failed",O1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="failed">
+      <formula>NOT(ISERROR(SEARCH("failed",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1817,28 +1875,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2">
         <v>150</v>
@@ -1850,12 +1908,12 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -1867,12 +1925,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -1884,12 +1942,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -1901,12 +1959,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1918,7 +1976,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1930,21 +1988,21 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1956,7 +2014,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -1968,12 +2026,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="2">
         <v>350</v>
@@ -1985,7 +2043,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1997,7 +2055,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2009,27 +2067,27 @@
       </c>
       <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -2038,23 +2096,23 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -2063,7 +2121,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add first (positive) Login test
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
-    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
+    <sheet sheetId="3" r:id="rId3" name="DataSetInteractionPages"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -72,7 +72,7 @@
             <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
-Expected Effect - displayed error message, displayed rows, etc.</t>
+Expected Effect - displayed (error/greeting) message, displayed rows, etc.</t>
         </r>
       </text>
     </comment>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="138">
   <si>
     <t>Key</t>
   </si>
@@ -213,9 +213,6 @@
     <t>TelephoneNumberField_Empty_ErrorMessage</t>
   </si>
   <si>
-    <t>TelephoneNumberField_TooShortNumber_ErrorMessage</t>
-  </si>
-  <si>
     <t>TelephoneNumberField_NonNumericalCharacters_ErrorMessage</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>Error: E-mailField must contain a valid email address</t>
   </si>
   <si>
-    <t>Error: E-mail address already exists</t>
-  </si>
-  <si>
     <t>* Invalid File</t>
   </si>
   <si>
@@ -330,9 +324,6 @@
     <t>* Fields do not match</t>
   </si>
   <si>
-    <t>EmailField_DuplicateEmail_ErrorMessage</t>
-  </si>
-  <si>
     <t>PictureField_InvalidFileFormat_ErrorMessage</t>
   </si>
   <si>
@@ -537,16 +528,61 @@
     <t>Fullname</t>
   </si>
   <si>
-    <t>&lt;Fullname@uniqueemail.com&gt;</t>
-  </si>
-  <si>
-    <t>&lt;unique generated per test suite&gt;</t>
-  </si>
-  <si>
     <t>article list</t>
   </si>
   <si>
     <t>at least one article exists</t>
+  </si>
+  <si>
+    <t>&lt;unique, generated per test&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Fullname&gt;@uniqueemail.com&gt;</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>User Login with valid credentials</t>
+  </si>
+  <si>
+    <t>login form - all</t>
+  </si>
+  <si>
+    <t>User Logoff</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>Logoff</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>Login_ValidCredentials_LoginSuccessful</t>
+  </si>
+  <si>
+    <t>Logoff_ClickLogoffLink_LogoffSuccessful</t>
+  </si>
+  <si>
+    <t>AssertLoginDisplayed</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>Log in</t>
   </si>
 </sst>
 </file>
@@ -626,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -642,6 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,14 +1041,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.90625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -1030,27 +1067,27 @@
     <col min="15" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1059,7 +1096,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -1068,32 +1105,32 @@
         <v>7</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row spans="1:15" outlineLevel="0" r="2">
       <c r="A2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
@@ -1111,23 +1148,23 @@
         <v>10</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>11</v>
@@ -1145,40 +1182,40 @@
         <v>10</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>103</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I4" t="s">
         <v>122</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>10</v>
@@ -1187,16 +1224,16 @@
         <v>10</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row spans="1:15" outlineLevel="0" r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1205,10 +1242,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>12</v>
@@ -1226,11 +1263,11 @@
         <v>10</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1239,10 +1276,10 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
@@ -1260,26 +1297,34 @@
         <v>10</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>31</v>
+    <row spans="1:15" outlineLevel="0" r="7">
+      <c r="A7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>8</v>
@@ -1293,12 +1338,17 @@
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M7" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row spans="1:15" outlineLevel="0" r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1307,13 +1357,13 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>8</v>
@@ -1328,11 +1378,11 @@
         <v>10</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1344,10 +1394,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>8</v>
@@ -1362,11 +1412,11 @@
         <v>10</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4">
@@ -1378,10 +1428,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>8</v>
@@ -1396,11 +1446,11 @@
         <v>10</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1412,10 +1462,10 @@
         <v>6</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="2" t="s">
@@ -1428,11 +1478,11 @@
         <v>10</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1444,13 +1494,13 @@
         <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>9</v>
@@ -1462,11 +1512,11 @@
         <v>10</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1478,13 +1528,13 @@
         <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>9</v>
@@ -1496,11 +1546,11 @@
         <v>10</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1512,13 +1562,13 @@
         <v>6</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>9</v>
@@ -1530,45 +1580,56 @@
         <v>10</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>33</v>
+    <row spans="1:15" outlineLevel="0" r="15">
+      <c r="A15" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
       <c r="K15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M15" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="O15" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:15" outlineLevel="0" r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1577,19 +1638,19 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>10</v>
@@ -1598,11 +1659,11 @@
         <v>10</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1614,10 +1675,10 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>8</v>
@@ -1630,11 +1691,11 @@
         <v>10</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="18">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4">
@@ -1646,10 +1707,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>8</v>
@@ -1658,17 +1719,17 @@
         <v>9</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1677,13 +1738,13 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>8</v>
@@ -1696,11 +1757,11 @@
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1709,13 +1770,13 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>8</v>
@@ -1727,14 +1788,14 @@
         <v>10</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1743,13 +1804,13 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>8</v>
@@ -1761,53 +1822,53 @@
         <v>10</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row spans="1:15" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1816,7 +1877,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1825,7 +1886,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row spans="1:15" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1875,28 +1936,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2">
         <v>150</v>
@@ -1908,12 +1969,12 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -1925,12 +1986,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -1942,12 +2003,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -1959,12 +2020,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1976,7 +2037,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1988,21 +2049,21 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2014,7 +2075,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -2026,12 +2087,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2">
         <v>350</v>
@@ -2043,7 +2104,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -2055,7 +2116,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2067,27 +2128,27 @@
       </c>
       <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -2096,23 +2157,23 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -2121,7 +2182,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
put 1 wait in RegisterPageMap
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1229,8 +1229,10 @@
       <c r="N4" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="O4" s="10" t="s">
-        <v>112</v>
+      <c r="O4" s="10" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
       </c>
     </row>
     <row spans="1:15" outlineLevel="0" r="5">
@@ -1344,8 +1346,10 @@
       <c r="N7" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="O7" s="11" t="s">
-        <v>112</v>
+      <c r="O7" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
       </c>
     </row>
     <row spans="1:15" outlineLevel="0" r="8">
@@ -1864,8 +1868,10 @@
       <c r="N22" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="O22" s="2" t="s">
-        <v>112</v>
+      <c r="O22" s="2" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
       </c>
     </row>
     <row spans="1:15" outlineLevel="0" r="23">

</xml_diff>

<commit_message>
Add first Create [Article] Test
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="141">
   <si>
     <t>Key</t>
   </si>
@@ -219,9 +219,6 @@
     <t>UsernameField_Empty_ErrorMessage</t>
   </si>
   <si>
-    <t>UsernameField_DuplicateUsername_ErrorMessage</t>
-  </si>
-  <si>
     <t>EmailField_Empty_ErrorMessage</t>
   </si>
   <si>
@@ -267,9 +264,6 @@
     <t>invalid characters</t>
   </si>
   <si>
-    <t>already registered</t>
-  </si>
-  <si>
     <t>invalid format - no @ or no '.' after @</t>
   </si>
   <si>
@@ -306,9 +300,6 @@
     <t>* Minimum 10 Digits starting with Country Code</t>
   </si>
   <si>
-    <t>Error: Username already exists</t>
-  </si>
-  <si>
     <t>* Invalid email address</t>
   </si>
   <si>
@@ -579,10 +570,28 @@
     <t>AssertLoginDisplayed</t>
   </si>
   <si>
-    <t>failed</t>
-  </si>
-  <si>
     <t>Log in</t>
+  </si>
+  <si>
+    <t>Create Article</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>User Create Article with valid input</t>
+  </si>
+  <si>
+    <t>create article - all</t>
+  </si>
+  <si>
+    <t>Create_ValidFieldEntries_ArticleCreated</t>
+  </si>
+  <si>
+    <t>ArticleBodyText</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Ut congue augue lacinia, tristique odio ut, porta velit. Cras rutrum dolor ligula, ac ornare lectus cursus sed.</t>
   </si>
 </sst>
 </file>
@@ -687,7 +696,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -701,7 +710,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1042,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1062,32 +1071,33 @@
     <col min="10" max="10" width="18.36328125" style="2" customWidth="1"/>
     <col min="11" max="11" width="9.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7265625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.453125" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="2"/>
+    <col min="13" max="13" width="15.81640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.7265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="16.453125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:15" outlineLevel="0" r="1">
+    <row spans="1:16" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1096,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -1104,33 +1114,36 @@
       <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>107</v>
+      <c r="M1" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="2">
+        <v>104</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="2">
       <c r="A2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
@@ -1147,24 +1160,24 @@
       <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="3">
+      <c r="N2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>11</v>
@@ -1181,61 +1194,59 @@
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="4">
+      <c r="N3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="H4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="O4" s="10" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="5">
+      <c r="O4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1244,10 +1255,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>12</v>
@@ -1264,12 +1275,12 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="6">
+      <c r="N5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1278,10 +1289,10 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
@@ -1298,35 +1309,35 @@
       <c r="L6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="7">
+      <c r="N6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="7">
       <c r="A7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>127</v>
-      </c>
       <c r="G7" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>8</v>
@@ -1340,19 +1351,17 @@
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="N7" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="O7" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="8">
+        <v>114</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1361,10 +1370,10 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
@@ -1381,12 +1390,12 @@
       <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="9">
+      <c r="N8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1398,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>15</v>
@@ -1415,27 +1424,35 @@
       <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>32</v>
+      <c r="N9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="10">
+      <c r="A10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>8</v>
@@ -1449,12 +1466,18 @@
       <c r="L10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>45</v>
+      <c r="M10" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="N10" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="11">
+      <c r="O10" s="4"/>
+      <c r="P10" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1466,10 +1489,10 @@
         <v>6</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="2" t="s">
@@ -1481,12 +1504,12 @@
       <c r="L11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N11" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="12">
+      <c r="N11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1498,13 +1521,13 @@
         <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>9</v>
@@ -1515,12 +1538,12 @@
       <c r="L12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N12" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="13">
+      <c r="N12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1532,13 +1555,13 @@
         <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>9</v>
@@ -1549,12 +1572,12 @@
       <c r="L13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N13" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="14">
+      <c r="N13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1566,13 +1589,13 @@
         <v>6</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>9</v>
@@ -1583,35 +1606,35 @@
       <c r="L14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N14" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="15">
+      <c r="N14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O14" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="H15" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1621,19 +1644,17 @@
       <c r="L15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="O15" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="16">
+      <c r="N15" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1642,19 +1663,19 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>10</v>
@@ -1662,12 +1683,12 @@
       <c r="L16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="N16" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="17">
+      <c r="N16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1679,10 +1700,10 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>8</v>
@@ -1694,12 +1715,12 @@
       <c r="L17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N17" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="18">
+      <c r="N17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="18">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4">
@@ -1711,10 +1732,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>8</v>
@@ -1723,17 +1744,17 @@
         <v>9</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N18" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="19">
+      <c r="N18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1742,13 +1763,13 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>8</v>
@@ -1760,12 +1781,13 @@
         <v>10</v>
       </c>
       <c r="L19" s="3"/>
-      <c r="M19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N19" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="20">
+      <c r="M19" s="3"/>
+      <c r="N19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1774,13 +1796,13 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>8</v>
@@ -1792,14 +1814,15 @@
         <v>10</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N20" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="21">
+        <v>55</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O20" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1808,13 +1831,13 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>8</v>
@@ -1826,55 +1849,55 @@
         <v>10</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="N21" s="4"/>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="22">
+        <v>55</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O21" s="4"/>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="M22" s="4"/>
       <c r="N22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="O22" s="2" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:15" outlineLevel="0" r="23">
+        <v>108</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1883,7 +1906,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row spans="1:15" outlineLevel="0" r="24">
+    <row spans="1:16" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1892,7 +1915,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row spans="1:15" outlineLevel="0" r="25">
+    <row spans="1:16" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1902,15 +1925,15 @@
       <c r="G25" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="failed">
-      <formula>NOT(ISERROR(SEARCH("failed",O1)))</formula>
+  <conditionalFormatting sqref="P1:P1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="failed">
+      <formula>NOT(ISERROR(SEARCH("failed",P1)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="failed">
-      <formula>NOT(ISERROR(SEARCH("failed",O1)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="failed">
+      <formula>NOT(ISERROR(SEARCH("failed",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1942,28 +1965,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2">
         <v>150</v>
@@ -1975,12 +1998,12 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -1992,12 +2015,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -2009,12 +2032,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -2026,12 +2049,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2043,7 +2066,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2055,21 +2078,21 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2081,7 +2104,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -2093,12 +2116,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B11" s="2">
         <v>350</v>
@@ -2110,7 +2133,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -2122,7 +2145,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2134,27 +2157,27 @@
       </c>
       <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -2163,23 +2186,23 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -2188,7 +2211,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix data-driven asserter call for Create Test[1]
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="143">
   <si>
     <t>Key</t>
   </si>
@@ -592,6 +592,12 @@
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Ut congue augue lacinia, tristique odio ut, porta velit. Cras rutrum dolor ligula, ac ornare lectus cursus sed.</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>AssertArticleIsDisplayed</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="O10" sqref="N10:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1469,8 +1475,12 @@
       <c r="M10" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="N10" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="P10" s="11" t="inlineStr">
         <is>
           <t>passed</t>

</xml_diff>

<commit_message>
Add first Edit [Article] test but with Thread.Sleep-s
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
-    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
-    <sheet sheetId="3" r:id="rId3" name="DataSetInteractionPages"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
+    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="147">
   <si>
     <t>Key</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Phone number</t>
   </si>
   <si>
-    <t>invalid length</t>
-  </si>
-  <si>
     <t>invalid characters</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t>* Invalid File</t>
   </si>
   <si>
-    <t>* Minimum 8 characters required</t>
-  </si>
-  <si>
     <t>* Fields do not match</t>
   </si>
   <si>
@@ -324,12 +318,6 @@
     <t>PassworField_Empty_ErrorMessage</t>
   </si>
   <si>
-    <t>shortPs</t>
-  </si>
-  <si>
-    <t>PassworField_TooShortPassword_ErrorMessage</t>
-  </si>
-  <si>
     <t>ConfirmPassworField_Empty_ErrorMessage</t>
   </si>
   <si>
@@ -598,6 +586,30 @@
   </si>
   <si>
     <t>AssertArticleIsDisplayed</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Edit Article</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>Author Edit Article</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Edited</t>
+  </si>
+  <si>
+    <t>Edit_ChangeContent_ContentChanged</t>
+  </si>
+  <si>
+    <t>AssertArticleIsEdited</t>
   </si>
 </sst>
 </file>
@@ -1056,14 +1068,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="O10" sqref="N10:O10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -1083,27 +1095,27 @@
     <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:16" outlineLevel="0" r="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="E1" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1112,7 +1124,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -1121,35 +1133,35 @@
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
@@ -1167,15 +1179,15 @@
         <v>10</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -1201,40 +1213,40 @@
         <v>10</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="F4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="I4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>10</v>
@@ -1243,16 +1255,16 @@
         <v>10</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1282,11 +1294,11 @@
         <v>10</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1316,34 +1328,34 @@
         <v>10</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="G7" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>8</v>
@@ -1358,16 +1370,16 @@
         <v>10</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1379,7 +1391,7 @@
         <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
@@ -1397,11 +1409,11 @@
         <v>10</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O8" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="9">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1431,34 +1443,34 @@
         <v>10</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O9" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="10">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>8</v>
@@ -1473,21 +1485,19 @@
         <v>10</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="P10" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="11">
+        <v>138</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1515,11 +1525,11 @@
         <v>10</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O11" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="12">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1531,7 +1541,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>17</v>
@@ -1549,11 +1559,11 @@
         <v>10</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O12" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="13">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1565,7 +1575,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>19</v>
@@ -1583,11 +1593,11 @@
         <v>10</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O13" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="14">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1599,7 +1609,7 @@
         <v>6</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>21</v>
@@ -1617,34 +1627,34 @@
         <v>10</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="H15" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1655,16 +1665,16 @@
         <v>10</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="16">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1673,19 +1683,19 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>10</v>
@@ -1694,11 +1704,11 @@
         <v>10</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="17">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1713,7 +1723,7 @@
         <v>24</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>8</v>
@@ -1726,26 +1736,34 @@
         <v>10</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O17" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="18">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>29</v>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>8</v>
@@ -1753,18 +1771,26 @@
       <c r="J18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>51</v>
+      <c r="K18" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" s="4"/>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="19">
+      <c r="M18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1773,13 +1799,13 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>8</v>
@@ -1793,11 +1819,11 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O19" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="20">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1806,13 +1832,13 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>8</v>
@@ -1824,15 +1850,15 @@
         <v>10</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="21">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1841,13 +1867,13 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>8</v>
@@ -1859,38 +1885,38 @@
         <v>10</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="22">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1898,16 +1924,16 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="23">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1916,7 +1942,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="24">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1925,7 +1951,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1975,28 +2001,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2">
         <v>150</v>
@@ -2008,12 +2034,12 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -2025,12 +2051,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -2042,12 +2068,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -2059,12 +2085,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2076,7 +2102,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2088,21 +2114,21 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2114,7 +2140,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -2126,12 +2152,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B11" s="2">
         <v>350</v>
@@ -2143,7 +2169,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -2155,7 +2181,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2167,27 +2193,27 @@
       </c>
       <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -2196,23 +2222,23 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -2221,7 +2247,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add few thread.sleep-s in Login and Logoff tests. Should be replaced with more intelligent wait
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
-    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
+    <sheet sheetId="3" r:id="rId3" name="DataSetInteractionPages"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -1068,10 +1068,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
@@ -1095,7 +1095,7 @@
     <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
       <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1260,11 +1260,13 @@
       <c r="O4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P4" s="10" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1298,7 +1300,7 @@
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1332,7 +1334,7 @@
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="7">
       <c r="A7" s="6" t="s">
         <v>116</v>
       </c>
@@ -1375,11 +1377,13 @@
       <c r="O7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P7" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P7" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1413,7 +1417,7 @@
       </c>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1447,7 +1451,7 @@
       </c>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="10">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -1493,11 +1497,13 @@
       <c r="O10" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="P10" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P10" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1529,7 +1535,7 @@
       </c>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1563,7 +1569,7 @@
       </c>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1597,7 +1603,7 @@
       </c>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1631,7 +1637,7 @@
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
         <v>122</v>
       </c>
@@ -1670,11 +1676,13 @@
       <c r="O15" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="P15" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P15" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1708,7 +1716,7 @@
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1740,7 +1748,7 @@
       </c>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="18">
       <c r="A18" s="6" t="s">
         <v>139</v>
       </c>
@@ -1786,11 +1794,13 @@
       <c r="O18" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="P18" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P18" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1823,7 +1833,7 @@
       </c>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1858,7 +1868,7 @@
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1893,7 +1903,7 @@
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
         <v>97</v>
       </c>
@@ -1929,11 +1939,13 @@
       <c r="O22" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P22" s="2" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1942,7 +1954,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1951,7 +1963,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>

</xml_diff>

<commit_message>
Add first Delete test, Change back to FF browser
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
-    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
-    <sheet sheetId="3" r:id="rId3" name="DataSetInteractionPages"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
+    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="154">
   <si>
     <t>Key</t>
   </si>
@@ -306,9 +306,6 @@
     <t>* Invalid File</t>
   </si>
   <si>
-    <t>* Fields do not match</t>
-  </si>
-  <si>
     <t>PictureField_InvalidFileFormat_ErrorMessage</t>
   </si>
   <si>
@@ -321,9 +318,6 @@
     <t>ConfirmPassworField_Empty_ErrorMessage</t>
   </si>
   <si>
-    <t>ConfirmPasswordField_NotMatchingPassword_ErrorMessage</t>
-  </si>
-  <si>
     <t>notMatchingConfirmPassString</t>
   </si>
   <si>
@@ -610,6 +604,33 @@
   </si>
   <si>
     <t>AssertArticleIsEdited</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Delete Article</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>Author Delete Article</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Delete_DeleteArticle_ArticleDeteted</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>AssertArticleIsDeleted</t>
   </si>
 </sst>
 </file>
@@ -657,18 +678,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -689,19 +704,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,11 +1082,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1095,26 +1109,26 @@
     <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="1">
-      <c r="A1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="7" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1124,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -1133,35 +1147,35 @@
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>101</v>
+        <v>133</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
-      <c r="A2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>113</v>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
@@ -1178,23 +1192,23 @@
       <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1212,72 +1226,70 @@
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
-      <c r="A4" s="6" t="s">
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="P4" s="10" t="inlineStr">
-        <is>
-          <t>failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
+      <c r="P4" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -1295,23 +1307,23 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
         <v>5</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1329,35 +1341,35 @@
       <c r="L6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="7">
-      <c r="A7" s="6" t="s">
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="D7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>93</v>
+      <c r="G7" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>8</v>
@@ -1371,30 +1383,28 @@
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="P7" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="8">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4">
+      <c r="N7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>7</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1412,23 +1422,23 @@
       <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="9">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4">
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
         <v>8</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -1446,107 +1456,106 @@
       <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O9" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="10">
-      <c r="A10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="P10" s="11" t="inlineStr">
-        <is>
-          <t>failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="11">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="P10" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="4" t="s">
+      <c r="K11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4">
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
         <v>11</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1555,32 +1564,33 @@
       <c r="I12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="4" t="s">
+      <c r="K12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O12" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="13">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4">
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -1589,32 +1599,33 @@
       <c r="I13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N13" s="4" t="s">
+      <c r="K13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="14">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4">
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
         <v>13</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1623,354 +1634,363 @@
       <c r="I14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N14" s="4" t="s">
+      <c r="K14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="15">
-      <c r="A15" s="6" t="s">
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="H15" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="P15" s="11" t="inlineStr">
-        <is>
-          <t>failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="16">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4">
+      <c r="O15" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
         <v>15</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="K16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O16" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="17">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="J17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O17" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="18">
-      <c r="A18" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="P18" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="19">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="4" t="s">
+      <c r="N19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O19" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="20">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="3" t="s">
+      <c r="K21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="21">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4">
-        <v>21</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O21" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="22">
-      <c r="A22" s="6" t="s">
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="D22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>106</v>
       </c>
+      <c r="G22" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="H22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="O22" s="6" t="s">
+      <c r="O22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P22" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P22" s="2" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="23">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="24">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P1:P1048576">
@@ -2009,32 +2029,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
-        <v>62</v>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2">
         <v>150</v>
@@ -2046,12 +2066,12 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -2063,12 +2083,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -2080,12 +2100,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -2097,12 +2117,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2114,7 +2134,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2126,21 +2146,21 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2152,7 +2172,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -2164,12 +2184,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2">
         <v>350</v>
@@ -2181,7 +2201,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -2193,7 +2213,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2205,27 +2225,27 @@
       </c>
       <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -2234,23 +2254,23 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
         <v>77</v>
-      </c>
-      <c r="H17" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -2259,7 +2279,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Negative tests + methods
Added the following negative tests:
-Register_Without_Email
-Register_Without_FullName
-Register_Without_Password
-Register_Without_ConfirmPassword

Added additional "Effect" & "Asserter" properties to BlogPages class to
accomodate two simultaneous error messages.
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
-    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
-    <sheet sheetId="3" r:id="rId3" name="DataSetInteractionPages"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
+    <sheet name="NegativeTests" sheetId="4" r:id="rId3"/>
+    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -24,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +113,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -138,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="166">
   <si>
     <t>Key</t>
   </si>
@@ -610,13 +611,70 @@
   </si>
   <si>
     <t>AssertArticleIsEdited</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>The Email field is required.</t>
+  </si>
+  <si>
+    <t>AssertEmailErrorMessageExists</t>
+  </si>
+  <si>
+    <t>Register_Without_Email</t>
+  </si>
+  <si>
+    <t>Register_Without_FullName</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>The Full Name field is required.</t>
+  </si>
+  <si>
+    <t>AssertFullNameErrorMessageExists</t>
+  </si>
+  <si>
+    <t>Effect2</t>
+  </si>
+  <si>
+    <t>Register_Without_Password</t>
+  </si>
+  <si>
+    <t>The Password field is required.</t>
+  </si>
+  <si>
+    <t>The password and confirmation password do not match.</t>
+  </si>
+  <si>
+    <t>Asserter2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AssertPasswordErrorMessageExists</t>
+  </si>
+  <si>
+    <t>AssertPasswordMissmatchErrorMessageExists</t>
+  </si>
+  <si>
+    <t>Register_Without_ConfirmPassword</t>
+  </si>
+  <si>
+    <t>AssertPasswordMissmatchErrorMessageExists2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +714,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -686,10 +752,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -706,8 +773,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -737,6 +806,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -785,7 +857,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -820,7 +892,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1035,12 +1107,12 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1068,34 +1140,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="42" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="46.26953125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="27.7265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="16.453125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="46.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="58.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="37.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -1145,7 +1217,7 @@
         <v>95</v>
       </c>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
@@ -1183,7 +1255,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1217,7 +1289,7 @@
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1260,13 +1332,11 @@
       <c r="O4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="10" t="inlineStr">
-        <is>
-          <t>failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
+      <c r="P4" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1300,7 +1370,7 @@
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1334,7 +1404,7 @@
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>116</v>
       </c>
@@ -1377,13 +1447,11 @@
       <c r="O7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P7" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="8">
+      <c r="P7" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1417,7 +1485,7 @@
       </c>
       <c r="O8" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="9">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1451,7 +1519,7 @@
       </c>
       <c r="O9" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="10">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -1497,13 +1565,11 @@
       <c r="O10" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="P10" s="11" t="inlineStr">
-        <is>
-          <t>failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="11">
+      <c r="P10" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1535,7 +1601,7 @@
       </c>
       <c r="O11" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="12">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1569,7 +1635,7 @@
       </c>
       <c r="O12" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="13">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1603,7 +1669,7 @@
       </c>
       <c r="O13" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="14">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1637,7 +1703,7 @@
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>122</v>
       </c>
@@ -1676,13 +1742,11 @@
       <c r="O15" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="P15" s="11" t="inlineStr">
-        <is>
-          <t>failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="16">
+      <c r="P15" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1716,7 +1780,7 @@
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="17">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1748,7 +1812,7 @@
       </c>
       <c r="O17" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="18">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>139</v>
       </c>
@@ -1794,13 +1858,11 @@
       <c r="O18" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="P18" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="19">
+      <c r="P18" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1833,7 +1895,7 @@
       </c>
       <c r="O19" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="20">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1868,7 +1930,7 @@
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="21">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1903,7 +1965,7 @@
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="22">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>97</v>
       </c>
@@ -1939,13 +2001,11 @@
       <c r="O22" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="P22" s="2" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="23">
+      <c r="P22" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1954,7 +2014,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="24">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1963,7 +2023,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row spans="1:16" x14ac:dyDescent="0.35" outlineLevel="0" r="25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1991,6 +2051,169 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
@@ -1998,17 +2221,17 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.26953125" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="24.26953125" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2255,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2049,7 +2272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2066,7 +2289,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2083,7 +2306,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -2100,7 +2323,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -2117,14 +2340,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -2143,14 +2366,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -2167,7 +2390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2184,14 +2407,14 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -2208,7 +2431,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2223,7 +2446,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -2237,7 +2460,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -2248,7 +2471,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Ran a few tests for good measure. Changes to text files.
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
-    <sheet name="NegativeTests" sheetId="4" r:id="rId3"/>
-    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId4"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
+    <sheet sheetId="4" r:id="rId3" name="NegativeTests"/>
+    <sheet sheetId="3" r:id="rId4" name="DataSetInteractionPages"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -1143,14 +1143,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
       <selection activeCell="J4" sqref="J4:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -1170,7 +1170,7 @@
     <col min="16" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="2">
       <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1335,11 +1335,13 @@
       <c r="O4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4" s="10" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1373,7 +1375,7 @@
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1407,7 +1409,7 @@
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="7">
       <c r="A7" s="6" t="s">
         <v>116</v>
       </c>
@@ -1454,7 +1456,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1488,7 +1490,7 @@
       </c>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1522,7 +1524,7 @@
       </c>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="10">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1604,7 +1606,7 @@
       </c>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1638,7 +1640,7 @@
       </c>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1672,7 +1674,7 @@
       </c>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1706,7 +1708,7 @@
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
         <v>122</v>
       </c>
@@ -1749,7 +1751,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1783,7 +1785,7 @@
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1815,7 +1817,7 @@
       </c>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="18">
       <c r="A18" s="6" t="s">
         <v>139</v>
       </c>
@@ -1865,7 +1867,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1898,7 +1900,7 @@
       </c>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1933,7 +1935,7 @@
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1968,7 +1970,7 @@
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
         <v>97</v>
       </c>
@@ -2008,7 +2010,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2017,7 +2019,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2026,7 +2028,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2054,14 +2056,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -2075,7 +2077,7 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row spans="1:10" outlineLevel="0" r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2107,7 +2109,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row spans="1:10" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
@@ -2126,11 +2128,13 @@
       <c r="H2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="3">
       <c r="A3" s="2" t="s">
         <v>152</v>
       </c>
@@ -2149,11 +2153,13 @@
       <c r="H3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="4">
       <c r="A4" s="2" t="s">
         <v>157</v>
       </c>
@@ -2181,11 +2187,13 @@
       <c r="I4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
         <v>164</v>
       </c>
@@ -2204,11 +2212,13 @@
       <c r="H5" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Several Changes. Hover above this for details.
1. Added twonegative test cases to the LoginPage test class:
-Login_InvalidPassword_LoginUnsuccessful
-Login_Blank_Email_Login_Unsuccessful

2. Added a test to RegisterPage test class meant to create a user for
our negative test cases:
-Setup_Negative_Test_Account

3. Refactored methods to avoid redundancies:
- RegisterPage.FillRegistrationFormNegative
- UserPage.FillRegistrationFormNegative

4. Added AccessExcelData.GetNegativeTestData and
AccessExcelData.WriteNegativeTestResult methods to accomodate second
data sheet usage.

5. Refactored the manner in which each tests saves its Status.
Functionality moved into the TearDown test class sections of
RegisterPage and LoginPage.
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
-    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
-    <sheet sheetId="4" r:id="rId3" name="NegativeTests"/>
-    <sheet sheetId="3" r:id="rId4" name="DataSetInteractionPages"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
+    <sheet name="NegativeTests" sheetId="4" r:id="rId3"/>
+    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="169">
   <si>
     <t>Key</t>
   </si>
@@ -671,6 +671,12 @@
   </si>
   <si>
     <t>Login_InvalidPassword_LoginUnsuccessful</t>
+  </si>
+  <si>
+    <t>Setup_Negative_Test_Account</t>
+  </si>
+  <si>
+    <t>Login_Blank_Email_Login_Unsuccessful</t>
   </si>
 </sst>
 </file>
@@ -1143,14 +1149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="J4" sqref="J4:N4"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -1170,7 +1176,7 @@
     <col min="16" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:16" outlineLevel="0" r="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>95</v>
       </c>
     </row>
-    <row spans="1:16" outlineLevel="0" r="2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
@@ -1258,7 +1264,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1292,7 +1298,7 @@
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1335,13 +1341,11 @@
       <c r="O4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="10" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="5">
+      <c r="P4" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1375,7 +1379,7 @@
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1409,7 +1413,7 @@
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>116</v>
       </c>
@@ -1456,7 +1460,7 @@
         <v>105</v>
       </c>
     </row>
-    <row spans="1:16" outlineLevel="0" r="8">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1490,7 +1494,7 @@
       </c>
       <c r="O8" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="9">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1524,7 +1528,7 @@
       </c>
       <c r="O9" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="10">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -1574,7 +1578,7 @@
         <v>147</v>
       </c>
     </row>
-    <row spans="1:16" outlineLevel="0" r="11">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1606,7 +1610,7 @@
       </c>
       <c r="O11" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="12">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1640,7 +1644,7 @@
       </c>
       <c r="O12" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="13">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1674,7 +1678,7 @@
       </c>
       <c r="O13" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="14">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1708,7 +1712,7 @@
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>122</v>
       </c>
@@ -1751,7 +1755,7 @@
         <v>147</v>
       </c>
     </row>
-    <row spans="1:16" outlineLevel="0" r="16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1785,7 +1789,7 @@
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="17">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1817,7 +1821,7 @@
       </c>
       <c r="O17" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="18">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>139</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>105</v>
       </c>
     </row>
-    <row spans="1:16" outlineLevel="0" r="19">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1900,7 +1904,7 @@
       </c>
       <c r="O19" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="20">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1935,7 +1939,7 @@
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="21">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1970,7 +1974,7 @@
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="22">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>97</v>
       </c>
@@ -2010,7 +2014,7 @@
         <v>105</v>
       </c>
     </row>
-    <row spans="1:16" outlineLevel="0" r="23">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2019,7 +2023,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="24">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2028,7 +2032,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2056,14 +2060,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -2077,7 +2081,7 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:10" outlineLevel="0" r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2109,7 +2113,7 @@
         <v>95</v>
       </c>
     </row>
-    <row spans="1:10" outlineLevel="0" r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
@@ -2128,13 +2132,11 @@
       <c r="H2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="3">
+      <c r="J2" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>152</v>
       </c>
@@ -2153,13 +2155,11 @@
       <c r="H3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J3" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="4">
+      <c r="J3" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>157</v>
       </c>
@@ -2187,13 +2187,11 @@
       <c r="I4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J4" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="5">
+      <c r="J4" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>164</v>
       </c>
@@ -2212,18 +2210,56 @@
       <c r="H5" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J5" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="6">
+      <c r="J5" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>153</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2232,9 +2268,10 @@
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes to database through tests. Read on...
Create_ValidFieldEntries_ArticleCreated test working properly.
Delete_DeleteArticle_ArticleDeteted test needs to have its test data
added to data source.
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
-    <sheet name="NegativeTests" sheetId="4" r:id="rId3"/>
-    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId4"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
+    <sheet sheetId="4" r:id="rId3" name="NegativeTests"/>
+    <sheet sheetId="3" r:id="rId4" name="DataSetInteractionPages"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -1149,14 +1149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -1176,7 +1176,7 @@
     <col min="16" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="1">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="2">
       <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1341,11 +1341,13 @@
       <c r="O4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4" s="10" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1379,7 +1381,7 @@
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1413,7 +1415,7 @@
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="7">
       <c r="A7" s="6" t="s">
         <v>116</v>
       </c>
@@ -1456,11 +1458,13 @@
       <c r="O7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P7" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1494,7 +1498,7 @@
       </c>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1528,7 +1532,7 @@
       </c>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="10">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -1574,11 +1578,13 @@
       <c r="O10" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="P10" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P10" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1610,7 +1616,7 @@
       </c>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1644,7 +1650,7 @@
       </c>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1678,7 +1684,7 @@
       </c>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1712,7 +1718,7 @@
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
         <v>122</v>
       </c>
@@ -1751,11 +1757,13 @@
       <c r="O15" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="P15" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P15" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1789,7 +1797,7 @@
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1821,7 +1829,7 @@
       </c>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="18">
       <c r="A18" s="6" t="s">
         <v>139</v>
       </c>
@@ -1867,11 +1875,13 @@
       <c r="O18" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="P18" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P18" s="11" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1904,7 +1914,7 @@
       </c>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1939,7 +1949,7 @@
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1974,7 +1984,7 @@
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
         <v>97</v>
       </c>
@@ -2010,11 +2020,13 @@
       <c r="O22" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P22" s="2" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2023,7 +2035,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2032,7 +2044,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2060,14 +2072,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -2081,7 +2093,7 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row spans="1:10" outlineLevel="0" r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2113,7 +2125,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row spans="1:10" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
@@ -2132,11 +2144,13 @@
       <c r="H2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="3">
       <c r="A3" s="2" t="s">
         <v>152</v>
       </c>
@@ -2155,11 +2169,13 @@
       <c r="H3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="4">
       <c r="A4" s="2" t="s">
         <v>157</v>
       </c>
@@ -2187,11 +2203,13 @@
       <c r="I4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
         <v>164</v>
       </c>
@@ -2210,11 +2228,13 @@
       <c r="H5" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
@@ -2230,8 +2250,13 @@
       <c r="H6" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="10" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="7">
       <c r="A7" s="2" t="s">
         <v>167</v>
       </c>
@@ -2247,8 +2272,13 @@
       <c r="E7" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="10" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
         <v>168</v>
       </c>
@@ -2260,6 +2290,11 @@
       </c>
       <c r="H8" s="2" t="s">
         <v>150</v>
+      </c>
+      <c r="J8" s="10" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved all negative tests into a separate class NegativeTests
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="169">
   <si>
     <t>Key</t>
   </si>
@@ -613,9 +613,6 @@
     <t>AssertArticleIsEdited</t>
   </si>
   <si>
-    <t>failed</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -677,6 +674,9 @@
   </si>
   <si>
     <t>Login_Blank_Email_Login_Unsuccessful</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -783,6 +783,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1149,14 +1158,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -1176,7 +1185,7 @@
     <col min="16" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:16" outlineLevel="0" r="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>95</v>
       </c>
     </row>
-    <row spans="1:16" outlineLevel="0" r="2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
@@ -1264,7 +1273,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1298,7 +1307,7 @@
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1341,13 +1350,11 @@
       <c r="O4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="5">
+      <c r="P4" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1381,7 +1388,7 @@
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1415,7 +1422,7 @@
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>116</v>
       </c>
@@ -1458,13 +1465,11 @@
       <c r="O7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P7" s="11" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="8">
+      <c r="P7" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
@@ -1498,7 +1503,7 @@
       </c>
       <c r="O8" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="9">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -1532,7 +1537,7 @@
       </c>
       <c r="O9" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="10">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -1578,13 +1583,11 @@
       <c r="O10" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="P10" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="11">
+      <c r="P10" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
@@ -1616,7 +1619,7 @@
       </c>
       <c r="O11" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="12">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -1650,7 +1653,7 @@
       </c>
       <c r="O12" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="13">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -1684,7 +1687,7 @@
       </c>
       <c r="O13" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="14">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
@@ -1718,7 +1721,7 @@
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>122</v>
       </c>
@@ -1757,13 +1760,11 @@
       <c r="O15" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="P15" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="16">
+      <c r="P15" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -1797,7 +1798,7 @@
       </c>
       <c r="O16" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="17">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
@@ -1829,7 +1830,7 @@
       </c>
       <c r="O17" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="18">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>139</v>
       </c>
@@ -1875,13 +1876,11 @@
       <c r="O18" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="P18" s="11" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="19">
+      <c r="P18" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
@@ -1914,7 +1913,7 @@
       </c>
       <c r="O19" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="20">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
@@ -1949,7 +1948,7 @@
       </c>
       <c r="O20" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="21">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
@@ -1984,7 +1983,7 @@
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="22">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>97</v>
       </c>
@@ -2020,13 +2019,11 @@
       <c r="O22" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="P22" s="2" t="inlineStr">
-        <is>
-          <t>passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:16" outlineLevel="0" r="23">
+      <c r="P22" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2035,7 +2032,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="24">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2044,7 +2041,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row spans="1:16" outlineLevel="0" r="25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2073,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2113,189 +2110,253 @@
         <v>100</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>101</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>95</v>
       </c>
     </row>
     <row spans="1:10" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J2" s="11" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="3">
-      <c r="A3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" s="11" t="inlineStr">
+      <c r="J2" s="15" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
       </c>
     </row>
-    <row spans="1:10" outlineLevel="0" r="4">
-      <c r="A4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="12" t="s">
+    <row spans="1:10" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="J4" s="11" t="inlineStr">
+      <c r="H3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J3" s="15" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
       </c>
     </row>
-    <row spans="1:10" outlineLevel="0" r="5">
-      <c r="A5" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J5" s="11" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="6">
-      <c r="A6" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="2" t="s">
+    <row spans="1:10" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J4" s="15" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
       </c>
     </row>
-    <row spans="1:10" outlineLevel="0" r="7">
-      <c r="A7" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="J7" s="10" t="inlineStr">
+    <row spans="1:10" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J5" s="15" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
       </c>
     </row>
-    <row spans="1:10" outlineLevel="0" r="8">
-      <c r="A8" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J8" s="10" t="inlineStr">
+    <row spans="1:10" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" s="13" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
       </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J8" s="13" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="9">
+      <c r="J9" s="14"/>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="10">
+      <c r="J10" s="14"/>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="11">
+      <c r="J11" s="14"/>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="12">
+      <c r="J12" s="14"/>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="13">
+      <c r="J13" s="14"/>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="14">
+      <c r="J14" s="14"/>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="15">
+      <c r="J15" s="14"/>
+    </row>
+    <row spans="1:10" outlineLevel="0" r="16">
+      <c r="J16" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="17">
+      <c r="J17" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="18">
+      <c r="J18" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="19">
+      <c r="J19" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="20">
+      <c r="J20" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="21">
+      <c r="J21" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="22">
+      <c r="J22" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="23">
+      <c r="J23" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="24">
+      <c r="J24" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="25">
+      <c r="J25" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="26">
+      <c r="J26" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="27">
+      <c r="J27" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="28">
+      <c r="J28" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="29">
+      <c r="J29" s="14"/>
+    </row>
+    <row spans="10:10" outlineLevel="0" r="30">
+      <c r="J30" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Correct USerData sheet in xls
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
-    <sheet sheetId="2" r:id="rId2" name="DataSet"/>
-    <sheet sheetId="4" r:id="rId3" name="NegativeTests"/>
-    <sheet sheetId="3" r:id="rId4" name="DataSetInteractionPages"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId2"/>
+    <sheet name="NegativeTests" sheetId="4" r:id="rId3"/>
+    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">DataSetInteractionPages!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -25,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0" shapeId="0">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="175">
   <si>
     <t>Key</t>
   </si>
@@ -307,9 +307,6 @@
     <t>* Invalid File</t>
   </si>
   <si>
-    <t>* Fields do not match</t>
-  </si>
-  <si>
     <t>PictureField_InvalidFileFormat_ErrorMessage</t>
   </si>
   <si>
@@ -322,9 +319,6 @@
     <t>ConfirmPassworField_Empty_ErrorMessage</t>
   </si>
   <si>
-    <t>ConfirmPasswordField_NotMatchingPassword_ErrorMessage</t>
-  </si>
-  <si>
     <t>notMatchingConfirmPassString</t>
   </si>
   <si>
@@ -677,6 +671,30 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Delete Article</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>Author Delete Article</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Delete_DeleteArticle_ArticleDeteted</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>AssertArticleIsDeleted</t>
   </si>
 </sst>
 </file>
@@ -732,18 +750,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -765,19 +777,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,7 +808,49 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -875,7 +928,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -910,7 +963,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1125,9 +1178,9 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1161,50 +1214,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="42" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="46.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="58.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="37.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.7109375" style="2"/>
+    <col min="6" max="6" width="18.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="46.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="58.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.7265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="37.54296875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="7" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1214,7 +1267,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -1223,35 +1276,35 @@
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>101</v>
+        <v>133</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>113</v>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
@@ -1268,23 +1321,23 @@
       <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1302,70 +1355,70 @@
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
+      <c r="P4" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -1383,23 +1436,23 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
         <v>5</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1417,35 +1470,35 @@
       <c r="L6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="D7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>93</v>
+      <c r="G7" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>8</v>
@@ -1459,28 +1512,28 @@
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4">
+      <c r="N7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>7</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1498,23 +1551,23 @@
       <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4">
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
         <v>8</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -1532,105 +1585,106 @@
       <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="P10" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="P10" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="4" t="s">
+      <c r="K11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4">
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
         <v>11</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1639,32 +1693,33 @@
       <c r="I12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="4" t="s">
+      <c r="K12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4">
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -1673,32 +1728,33 @@
       <c r="I13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N13" s="4" t="s">
+      <c r="K13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4">
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
         <v>13</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1707,358 +1763,386 @@
       <c r="I14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N14" s="4" t="s">
+      <c r="K14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="H15" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="P15" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4">
+      <c r="O15" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
         <v>15</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="K16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="J17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="P18" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="4" t="s">
+      <c r="N19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="3" t="s">
+      <c r="K21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4">
-        <v>21</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="D22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>106</v>
       </c>
+      <c r="G22" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="H22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="O22" s="6" t="s">
+      <c r="O22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P22" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="failed">
+  <conditionalFormatting sqref="P23:P1048576">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="failed">
+      <formula>NOT(ISERROR(SEARCH("failed",P23)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="failed">
+      <formula>NOT(ISERROR(SEARCH("failed",P23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P22">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="failed">
       <formula>NOT(ISERROR(SEARCH("failed",P1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="failed">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="failed">
       <formula>NOT(ISERROR(SEARCH("failed",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2069,28 +2153,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="30.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="2"/>
+    <col min="5" max="5" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:10" outlineLevel="0" r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2182,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2107,256 +2191,244 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" s="15" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="3">
-      <c r="A3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J3" s="15" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="4">
-      <c r="A4" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="J4" s="15" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="5">
-      <c r="A5" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="J5" s="15" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="6">
-      <c r="A6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J6" s="13" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="7">
-      <c r="A7" s="2" t="s">
+      <c r="J8" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="8">
-      <c r="A8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="J8" s="13" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="9">
-      <c r="J9" s="14"/>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="10">
-      <c r="J10" s="14"/>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="11">
-      <c r="J11" s="14"/>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="12">
-      <c r="J12" s="14"/>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="13">
-      <c r="J13" s="14"/>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="14">
-      <c r="J14" s="14"/>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="15">
-      <c r="J15" s="14"/>
-    </row>
-    <row spans="1:10" outlineLevel="0" r="16">
-      <c r="J16" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="17">
-      <c r="J17" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="18">
-      <c r="J18" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="19">
-      <c r="J19" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="20">
-      <c r="J20" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="21">
-      <c r="J21" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="22">
-      <c r="J22" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="23">
-      <c r="J23" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="24">
-      <c r="J24" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="25">
-      <c r="J25" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="26">
-      <c r="J26" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="27">
-      <c r="J27" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="28">
-      <c r="J28" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="29">
-      <c r="J29" s="14"/>
-    </row>
-    <row spans="10:10" outlineLevel="0" r="30">
-      <c r="J30" s="14"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J30" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2379,43 +2451,43 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2">
         <v>150</v>
@@ -2427,12 +2499,12 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -2444,12 +2516,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -2461,12 +2533,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -2478,12 +2550,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2495,45 +2567,45 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="H8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -2545,12 +2617,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2">
         <v>350</v>
@@ -2562,19 +2634,19 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2586,27 +2658,27 @@
       </c>
       <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -2615,23 +2687,23 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>81</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -2640,7 +2712,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move Old Failed Tests Logger to BasePage
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,13 +7,13 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="DataSet" sheetId="2" r:id="rId1"/>
-    <sheet name="NegativeTests" sheetId="4" r:id="rId2"/>
+    <sheet sheetId="2" r:id="rId1" name="DataSet"/>
+    <sheet sheetId="4" r:id="rId2" name="NegativeTests"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -904,14 +904,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -932,7 +932,7 @@
     <col min="18" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="1">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -988,7 +988,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="2">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -1054,7 +1054,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -1138,7 +1138,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="6">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1171,7 +1171,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="7">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1210,7 +1210,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="8">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -1245,7 +1245,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="9">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1274,7 +1274,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -1351,7 +1351,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="12">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -1385,7 +1385,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="13">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1431,11 +1431,13 @@
         <v>72</v>
       </c>
       <c r="Q13" s="5"/>
-      <c r="R13" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R13" s="8" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="14">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
@@ -1459,7 +1461,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -1483,7 +1485,7 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="16">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -1507,7 +1509,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="17">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -1531,7 +1533,7 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="18">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
@@ -1577,7 +1579,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="19">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -1603,7 +1605,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="20">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -1627,7 +1629,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="21">
       <c r="A21" s="5" t="s">
         <v>73</v>
       </c>
@@ -1677,7 +1679,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="22">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -1701,7 +1703,7 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="23">
       <c r="A23" s="5" t="s">
         <v>103</v>
       </c>
@@ -1749,7 +1751,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="24">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3">
@@ -1775,7 +1777,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="25">
       <c r="A25" s="5" t="s">
         <v>32</v>
       </c>
@@ -1817,7 +1819,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="26">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1826,7 +1828,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1835,7 +1837,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row spans="1:18" outlineLevel="0" r="28">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>

</xml_diff>

<commit_message>
Read for full description
Removed NegativeTests test class.
All methods move to their respective pages.
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1101,7 +1101,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="10" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="R5" s="10" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="R6" s="10" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="R7" s="10" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="R8" s="10" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="8" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1363,7 +1363,7 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="10" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="10" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="8" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="8" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="8" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       <c r="Q23" s="5"/>
       <c r="R23" s="8" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
       <c r="Q25" s="5"/>
       <c r="R25" s="8" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Inconclusive</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
See description for changelog
Added following navigation tests:
Home_ClickLogin_LoginLoaded
Home_ClickRegister_RegisterLoaded
Home_LogoClick_HomePageLoaded
Manage_ClickAccount_NavigateToManagePage
Create_CreateArticleCancelButton_NavigateToHomePage
Home_CreateArticle_ReadArticle
Delete_ClickDeleteButton_ConfirmationPageLoaded
Edit_ClickEdit_EditPageLoaded
Home_ClickOnAccount_ManagePageLoaded

Renamed some tests;
Reworked some tests descriptions;
Added ManagePage class and PoM;
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="2" r:id="rId1" name="DataSet"/>
-    <sheet sheetId="4" r:id="rId2" name="NegativeTests"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId1"/>
+    <sheet name="NegativeTests" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -23,7 +23,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="141">
   <si>
     <t>Key</t>
   </si>
@@ -448,6 +448,87 @@
   </si>
   <si>
     <t>Failed</t>
+  </si>
+  <si>
+    <t>http://localhost:60639/Account/Login</t>
+  </si>
+  <si>
+    <t>Navigate to Register page</t>
+  </si>
+  <si>
+    <t>Navigate to Log in page</t>
+  </si>
+  <si>
+    <t>http://localhost:60639/Account/Register</t>
+  </si>
+  <si>
+    <t>http://localhost:60639/Article/List</t>
+  </si>
+  <si>
+    <t>Navigate to Home page throuhg Logo link</t>
+  </si>
+  <si>
+    <t>http://localhost:60639/Manage</t>
+  </si>
+  <si>
+    <t>Log in and enter Account Management</t>
+  </si>
+  <si>
+    <t>Navigate to create article and click Cancel</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Log in and read an article</t>
+  </si>
+  <si>
+    <t>Manage_ClickAccount_NavigateToManagePage</t>
+  </si>
+  <si>
+    <t>Create_CreateArticleCancelButton_NavigateToHomePage</t>
+  </si>
+  <si>
+    <t>Delete_ClickDeleteButton_ConfirmationPageLoaded</t>
+  </si>
+  <si>
+    <t>Edit_ClickEdit_EditPageLoaded</t>
+  </si>
+  <si>
+    <t>Home_ClickOnAccount_ManagePageLoaded</t>
+  </si>
+  <si>
+    <t>Home_ClickLogin_LoginLoaded</t>
+  </si>
+  <si>
+    <t>Home_ClickRegister_RegisterLoaded</t>
+  </si>
+  <si>
+    <t>Home_CreateArticle_ReadArticle</t>
+  </si>
+  <si>
+    <t>Home_LogoClick_HomePageLoaded</t>
+  </si>
+  <si>
+    <t>Log in and select article to edit</t>
+  </si>
+  <si>
+    <t>Log in and navigate to manage page</t>
+  </si>
+  <si>
+    <t>Log in and select article to delete</t>
+  </si>
+  <si>
+    <t>Attempt registration without email</t>
+  </si>
+  <si>
+    <t>Attempt registration without full name</t>
+  </si>
+  <si>
+    <t>Attempt registration without password</t>
+  </si>
+  <si>
+    <t>Attempt registration without confirm password</t>
   </si>
 </sst>
 </file>
@@ -536,12 +617,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -562,28 +642,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -661,7 +720,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,7 +755,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -904,54 +963,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:R28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="42" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="46.26953125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="28.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.1796875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="27.7265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="26.54296875" style="2" customWidth="1"/>
-    <col min="16" max="17" width="37.54296875" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="46.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="26.5703125" style="2" customWidth="1"/>
+    <col min="16" max="17" width="37.5703125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:18" outlineLevel="0" r="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -972,38 +1031,38 @@
       <c r="M1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>93</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row spans="1:18" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1025,7 +1084,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row spans="1:18" outlineLevel="0" r="3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -1054,32 +1113,32 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row spans="1:18" outlineLevel="0" r="4">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1091,21 +1150,19 @@
       <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5" t="s">
+      <c r="O4" s="4"/>
+      <c r="P4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="5">
+      <c r="Q4" s="4"/>
+      <c r="R4" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -1113,14 +1170,14 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="2" t="s">
         <v>112</v>
       </c>
@@ -1136,19 +1193,17 @@
       <c r="P5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R5" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="6">
+      <c r="R5" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1158,7 +1213,7 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="13"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1171,19 +1226,17 @@
       <c r="P6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="R6" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="7">
+      <c r="R6" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1196,7 +1249,7 @@
       <c r="J7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="K7" s="13"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1212,13 +1265,11 @@
       <c r="Q7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="R7" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="8">
+      <c r="R7" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -1226,7 +1277,7 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1242,195 +1293,189 @@
       <c r="K8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="13"/>
+      <c r="L8" s="12"/>
       <c r="N8" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="9">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="R8" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="H9" s="2" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="K9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R9" s="10" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="10">
-      <c r="A10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="N9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="11">
+      <c r="K10" s="12"/>
+      <c r="N10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="13"/>
+        <v>101</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="K11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="N11" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="R11" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="H12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="K12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O12" s="3"/>
-      <c r="P12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="10" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="13">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
         <v>6</v>
@@ -1438,28 +1483,17 @@
       <c r="L13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="14">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1479,11 +1513,11 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row spans="1:18" outlineLevel="0" r="15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1503,11 +1537,11 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row spans="1:18" outlineLevel="0" r="16">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1527,16 +1561,31 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row spans="1:18" outlineLevel="0" r="17">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
@@ -1546,36 +1595,28 @@
         <v>6</v>
       </c>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="18">
-      <c r="A18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="N17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
@@ -1585,25 +1626,18 @@
         <v>6</v>
       </c>
       <c r="M18" s="3"/>
-      <c r="N18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="19">
+      <c r="N18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1611,293 +1645,474 @@
       <c r="G19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row spans="1:18" outlineLevel="0" r="20">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3">
-        <v>17</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="L20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="21">
-      <c r="A21" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="M20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
         <v>19</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="22">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3">
-        <v>19</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="23">
-      <c r="A23" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="L22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
+        <v>21</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="24">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3">
-        <v>21</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="25">
-      <c r="A25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="N24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="8" t="inlineStr">
-        <is>
-          <t>Inconclusive</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="26">
+        <v>130</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="N25" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="O25" s="3"/>
+      <c r="P25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="27">
+      <c r="E26" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="28">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="H27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R28" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R30" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="P31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R32" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="R26:R1048576">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="failed">
-      <formula>NOT(ISERROR(SEARCH("failed",R26)))</formula>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="failed">
+      <formula>NOT(ISERROR(SEARCH("failed",R1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="failed">
-      <formula>NOT(ISERROR(SEARCH("failed",R26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R25">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="failed">
-      <formula>NOT(ISERROR(SEARCH("failed",R1)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"passed"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="failed">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="failed">
       <formula>NOT(ISERROR(SEARCH("failed",R1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="N25" r:id="rId1"/>
+    <hyperlink ref="N26" r:id="rId2"/>
+    <hyperlink ref="N27" r:id="rId3"/>
+    <hyperlink ref="N28" r:id="rId4"/>
+    <hyperlink ref="N29" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1909,21 +2124,21 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="2"/>
-    <col min="5" max="5" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1951,11 +2166,11 @@
       <c r="I1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -1974,15 +2189,15 @@
       <c r="H2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1997,15 +2212,15 @@
       <c r="H3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2029,15 +2244,15 @@
       <c r="I4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2052,15 +2267,15 @@
       <c r="H5" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2072,15 +2287,15 @@
       <c r="H6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2092,11 +2307,11 @@
       <c r="E7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>101</v>
       </c>
@@ -2109,75 +2324,75 @@
       <c r="H8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J22" s="11"/>
-    </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J25" s="11"/>
-    </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J29" s="11"/>
-    </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J30" s="11"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Fix some failing tests (mainly waits); regular commit
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="DataSet" sheetId="2" r:id="rId1"/>
-    <sheet name="NegativeTests" sheetId="4" r:id="rId2"/>
+    <sheet sheetId="2" r:id="rId1" name="DataSet"/>
+    <sheet sheetId="4" r:id="rId2" name="NegativeTests"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -960,14 +960,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
       <selection activeCell="H25" sqref="H25:H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -988,7 +988,7 @@
     <col min="18" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="2">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -1110,7 +1110,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="4">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1155,11 +1155,13 @@
         <v>43</v>
       </c>
       <c r="Q4" s="4"/>
-      <c r="R4" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -1190,11 +1192,13 @@
       <c r="P5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R5" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="6">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1223,11 +1227,13 @@
       <c r="P6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="R6" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="7">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1262,11 +1268,13 @@
       <c r="Q7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="R7" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="8">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -1297,11 +1305,13 @@
       <c r="P8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="9">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
@@ -1343,11 +1353,13 @@
         <v>43</v>
       </c>
       <c r="Q9" s="4"/>
-      <c r="R9" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="10">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -1374,11 +1386,13 @@
         <v>95</v>
       </c>
       <c r="Q10" s="3"/>
-      <c r="R10" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -1408,11 +1422,13 @@
         <v>83</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="11" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1458,11 +1474,13 @@
         <v>72</v>
       </c>
       <c r="Q12" s="4"/>
-      <c r="R12" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="13">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -1486,7 +1504,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="14">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
@@ -1510,7 +1528,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -1534,7 +1552,7 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="16">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -1558,7 +1576,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="17">
       <c r="A17" s="4" t="s">
         <v>56</v>
       </c>
@@ -1600,11 +1618,13 @@
         <v>62</v>
       </c>
       <c r="Q17" s="4"/>
-      <c r="R17" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="18">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -1630,7 +1650,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="19">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -1654,7 +1674,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="20">
       <c r="A20" s="4" t="s">
         <v>73</v>
       </c>
@@ -1700,11 +1720,13 @@
         <v>80</v>
       </c>
       <c r="Q20" s="4"/>
-      <c r="R20" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="21">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -1728,7 +1750,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="22">
       <c r="A22" s="4" t="s">
         <v>103</v>
       </c>
@@ -1772,11 +1794,13 @@
         <v>110</v>
       </c>
       <c r="Q22" s="4"/>
-      <c r="R22" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R22" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="23">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
@@ -1802,7 +1826,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row spans="1:18" outlineLevel="0" r="24">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
@@ -1840,11 +1864,13 @@
         <v>38</v>
       </c>
       <c r="Q24" s="4"/>
-      <c r="R24" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="7" t="inlineStr">
+        <is>
+          <t>Inconclusive</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1866,11 +1892,13 @@
         <v>122</v>
       </c>
       <c r="Q25" s="3"/>
-      <c r="R25" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R25" s="11" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="26">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1889,11 +1917,13 @@
       <c r="P26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R26" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="7" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1912,11 +1942,13 @@
       <c r="P27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R27" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R27" s="7" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="28">
       <c r="E28" s="2" t="s">
         <v>120</v>
       </c>
@@ -1941,11 +1973,13 @@
       <c r="P28" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R28" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R28" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="29">
       <c r="E29" s="2" t="s">
         <v>121</v>
       </c>
@@ -1970,11 +2004,13 @@
       <c r="P29" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R29" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R29" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="30">
       <c r="E30" s="2" t="s">
         <v>123</v>
       </c>
@@ -2002,11 +2038,13 @@
       <c r="P30" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R30" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R30" s="7" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="31">
       <c r="E31" s="2" t="s">
         <v>135</v>
       </c>
@@ -2032,11 +2070,13 @@
       <c r="P31" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R31" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R31" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:18" outlineLevel="0" r="32">
       <c r="E32" s="2" t="s">
         <v>133</v>
       </c>
@@ -2058,11 +2098,13 @@
       <c r="P32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R32" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="R32" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
+    <row spans="5:18" outlineLevel="0" r="33">
       <c r="E33" s="2" t="s">
         <v>134</v>
       </c>
@@ -2084,8 +2126,10 @@
       <c r="P33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R33" s="7" t="s">
-        <v>102</v>
+      <c r="R33" s="7" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored some tests to work with the data driven asserter
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="174">
   <si>
     <t>Key</t>
   </si>
@@ -467,9 +467,6 @@
     <t>Log in and select article to delete</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
     <t>Register Account without Email</t>
   </si>
   <si>
@@ -606,6 +603,30 @@
   </si>
   <si>
     <t>Account_ClickOnChangePassword_ChangePasswordPageLoaded</t>
+  </si>
+  <si>
+    <t>AssertLoginPageUrl</t>
+  </si>
+  <si>
+    <t>AssertRegisterPageUrl</t>
+  </si>
+  <si>
+    <t>AssertHomePageUrl</t>
+  </si>
+  <si>
+    <t>AssertChangePasswordDisplayed</t>
+  </si>
+  <si>
+    <t>Change your password</t>
+  </si>
+  <si>
+    <t>AssertManagePageUrl</t>
+  </si>
+  <si>
+    <t>AssertConfirmDeleteButtonDisplayed</t>
+  </si>
+  <si>
+    <t>http://localhost:60639/Article/Delete/</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,19 +1206,19 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>75</v>
@@ -1226,19 +1247,19 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>76</v>
@@ -1267,19 +1288,19 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>80</v>
@@ -1314,19 +1335,19 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>86</v>
@@ -1404,22 +1425,22 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>4</v>
@@ -1447,19 +1468,19 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>88</v>
@@ -1490,19 +1511,19 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I11" s="9"/>
       <c r="O11" s="3"/>
@@ -1565,19 +1586,19 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1597,19 +1618,19 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>69</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1629,19 +1650,19 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1855,13 +1876,13 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>6</v>
@@ -1880,18 +1901,18 @@
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="2" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="8" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>6</v>
@@ -1908,23 +1929,23 @@
         <v>103</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1935,15 +1956,15 @@
         <v>104</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
@@ -1969,8 +1990,14 @@
       <c r="N23" t="s">
         <v>105</v>
       </c>
+      <c r="O23" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="P23" s="2" t="s">
-        <v>108</v>
+        <v>171</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="R23" s="7" t="s">
         <v>89</v>
@@ -1978,7 +2005,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>6</v>
@@ -2005,7 +2032,7 @@
         <v>104</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="R24" s="7" t="s">
         <v>89</v>
@@ -2013,7 +2040,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>6</v>
@@ -2046,12 +2073,12 @@
         <v>64</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>6</v>
@@ -2077,9 +2104,11 @@
       <c r="M26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N26" s="4"/>
+      <c r="N26" t="s">
+        <v>173</v>
+      </c>
       <c r="P26" s="2" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="R26" s="7" t="s">
         <v>89</v>
@@ -2087,7 +2116,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>6</v>
@@ -2119,16 +2148,16 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>41</v>
@@ -2149,20 +2178,20 @@
         <v>108</v>
       </c>
       <c r="R28" s="7" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
@@ -2170,7 +2199,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -2178,7 +2207,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Forgot to close some associated files. Trash commit.
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="220">
   <si>
     <t>Key</t>
   </si>
@@ -701,9 +701,6 @@
     <t>Click</t>
   </si>
   <si>
-    <t>Create_CommentArticle_CommentButtonExists</t>
-  </si>
-  <si>
     <t>AssertCommentButtonExists</t>
   </si>
   <si>
@@ -743,9 +740,6 @@
     <t>AssertUnableToEditMessageExists</t>
   </si>
   <si>
-    <t>Unable to edit other Author's articles</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -756,6 +750,21 @@
   </si>
   <si>
     <t>User Login with invalid Email format</t>
+  </si>
+  <si>
+    <t>AssertCommentCreatedSuccessfully</t>
+  </si>
+  <si>
+    <t>Comment_CommentAnArticle_CommentCreated</t>
+  </si>
+  <si>
+    <t>Comment_CommentArticle_CommentButtonExists</t>
+  </si>
+  <si>
+    <t>Comment by:</t>
+  </si>
+  <si>
+    <t>Unable to edit other Authors articles</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1186,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1700,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>188</v>
@@ -1916,34 +1925,55 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="H17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="3" t="s">
+        <v>215</v>
+      </c>
       <c r="Q17" s="3"/>
-      <c r="R17" s="7"/>
+      <c r="R17" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2051,22 +2081,22 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>197</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>41</v>
@@ -2082,11 +2112,11 @@
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="4" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="7" t="s">
@@ -2511,7 +2541,7 @@
         <v>197</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>41</v>
@@ -2529,10 +2559,10 @@
         <v>62</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R32" s="7" t="s">
         <v>176</v>
@@ -2540,22 +2570,22 @@
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>149</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>41</v>
@@ -2573,10 +2603,10 @@
         <v>62</v>
       </c>
       <c r="N33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="P33" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Adjust tests priorities and properties, AAA, proofread
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet sheetId="2" r:id="rId1" name="DataSet"/>
@@ -22,7 +22,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="222">
   <si>
     <t>Key</t>
   </si>
@@ -371,9 +371,6 @@
     <t>AssertPasswordMissmatchErrorMessageExists2</t>
   </si>
   <si>
-    <t>Login_Blank_Email_Login_Unsuccessful</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
@@ -425,18 +422,9 @@
     <t>http://localhost:60639/Manage</t>
   </si>
   <si>
-    <t>Log in and enter Account Management</t>
-  </si>
-  <si>
-    <t>Navigate to create article and click Cancel</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
-    <t>Log in and read an article</t>
-  </si>
-  <si>
     <t>Manage_ClickAccount_NavigateToManagePage</t>
   </si>
   <si>
@@ -461,12 +449,6 @@
     <t>Home_LogoClick_HomePageLoaded</t>
   </si>
   <si>
-    <t>Log in and select article to edit</t>
-  </si>
-  <si>
-    <t>Log in and select article to delete</t>
-  </si>
-  <si>
     <t>Register Account without Email</t>
   </si>
   <si>
@@ -599,9 +581,6 @@
     <t>Navigate to Home page through Logo link</t>
   </si>
   <si>
-    <t>Log in and navigate to passwod change page</t>
-  </si>
-  <si>
     <t>Account_ClickOnChangePassword_ChangePasswordPageLoaded</t>
   </si>
   <si>
@@ -659,9 +638,6 @@
     <t>3.3</t>
   </si>
   <si>
-    <t>Passwrd</t>
-  </si>
-  <si>
     <t>Login_WithInvalidPassword_LoginUnsuccessful</t>
   </si>
   <si>
@@ -692,9 +668,6 @@
     <t>10.10</t>
   </si>
   <si>
-    <t>Log in and comment created article</t>
-  </si>
-  <si>
     <t>Comment Button</t>
   </si>
   <si>
@@ -713,9 +686,6 @@
     <t xml:space="preserve">View article Author </t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>Create_NavigateToArticle_ArticleAuthorExists</t>
   </si>
   <si>
@@ -765,6 +735,42 @@
   </si>
   <si>
     <t>Unable to edit other Authors articles</t>
+  </si>
+  <si>
+    <t>Smoke tests</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Change password link</t>
+  </si>
+  <si>
+    <t>Log in and comment created Article</t>
+  </si>
+  <si>
+    <t>Log In and Select Article to Edit</t>
+  </si>
+  <si>
+    <t>Log In and Select Article to Delete</t>
+  </si>
+  <si>
+    <t>Log In and Read an Article</t>
+  </si>
+  <si>
+    <t>Navigate to Create Article and click Cancel</t>
+  </si>
+  <si>
+    <t>Log In and Enter Account Management</t>
+  </si>
+  <si>
+    <t>= positive tests - regression/smoke</t>
+  </si>
+  <si>
+    <t>Log In and navigate to Password change Page</t>
+  </si>
+  <si>
+    <t>Login_BlankEmail_Login_Unsuccessful</t>
   </si>
 </sst>
 </file>
@@ -939,7 +945,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -974,7 +980,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1183,31 +1189,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="42" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="46.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="26.5703125" style="2" customWidth="1"/>
-    <col min="16" max="17" width="37.5703125" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="8.7109375" style="2"/>
+    <col min="6" max="6" width="18.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="46.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.7265625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.1796875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.7265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="26.54296875" style="2" customWidth="1"/>
+    <col min="16" max="17" width="37.54296875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row spans="1:18" outlineLevel="0" r="1">
@@ -1346,26 +1352,26 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>75</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>5</v>
@@ -1389,19 +1395,19 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>76</v>
@@ -1432,19 +1438,19 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>80</v>
@@ -1453,7 +1459,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="2" t="s">
@@ -1481,19 +1487,19 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>86</v>
@@ -1502,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>5</v>
@@ -1575,28 +1581,28 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="2" t="s">
@@ -1620,22 +1626,22 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>184</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>41</v>
@@ -1643,18 +1649,18 @@
       <c r="J10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="8" t="inlineStr">
@@ -1667,26 +1673,26 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>88</v>
+        <v>221</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>5</v>
@@ -1712,35 +1718,35 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="I12" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="8" t="inlineStr">
@@ -1807,22 +1813,22 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>41</v>
@@ -1840,11 +1846,11 @@
         <v>62</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="7" t="inlineStr">
@@ -1857,22 +1863,22 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>69</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>41</v>
@@ -1886,13 +1892,13 @@
       <c r="L15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="3"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="7" t="inlineStr">
@@ -1905,22 +1911,22 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>41</v>
@@ -1938,11 +1944,11 @@
         <v>62</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="7" t="inlineStr">
@@ -1952,29 +1958,29 @@
       </c>
     </row>
     <row spans="1:18" outlineLevel="0" r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="E17" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>41</v>
@@ -1991,14 +1997,14 @@
       <c r="M17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q17" s="3"/>
+      <c r="N17" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q17" s="4"/>
       <c r="R17" s="7" t="inlineStr">
         <is>
           <t>Failed</t>
@@ -2068,7 +2074,7 @@
         <v>67</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>68</v>
@@ -2112,25 +2118,25 @@
       </c>
     </row>
     <row spans="1:18" outlineLevel="0" r="20">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>197</v>
       </c>
+      <c r="F20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="H20" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>41</v>
@@ -2145,14 +2151,14 @@
         <v>5</v>
       </c>
       <c r="M20" s="3"/>
-      <c r="N20" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q20" s="4"/>
+      <c r="N20" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q20" s="3"/>
       <c r="R20" s="7" t="inlineStr">
         <is>
           <t>Failed</t>
@@ -2161,28 +2167,28 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="21">
       <c r="A21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>63</v>
       </c>
       <c r="G21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>41</v>
@@ -2200,11 +2206,11 @@
         <v>62</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q21" s="4"/>
       <c r="R21" s="7" t="inlineStr">
@@ -2259,32 +2265,32 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="23">
       <c r="A23" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I23" s="9"/>
       <c r="N23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="8" t="inlineStr">
@@ -2297,24 +2303,24 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="N24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="R24" s="7" t="inlineStr">
         <is>
@@ -2326,24 +2332,24 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="N25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="R25" s="7" t="inlineStr">
         <is>
@@ -2353,16 +2359,16 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="26">
       <c r="C26" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>41</v>
@@ -2377,35 +2383,35 @@
         <v>5</v>
       </c>
       <c r="N26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="R26" s="7" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
     </row>
     <row spans="1:18" outlineLevel="0" r="27">
       <c r="C27" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>41</v>
@@ -2420,10 +2426,10 @@
         <v>5</v>
       </c>
       <c r="N27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="R27" s="7" t="inlineStr">
         <is>
@@ -2433,16 +2439,16 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="28">
       <c r="C28" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>109</v>
+        <v>216</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>41</v>
@@ -2459,7 +2465,7 @@
       <c r="M28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="N28" s="3" t="s">
         <v>63</v>
       </c>
       <c r="P28" s="2" t="s">
@@ -2473,16 +2479,16 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="29">
       <c r="C29" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>41</v>
@@ -2500,10 +2506,10 @@
         <v>62</v>
       </c>
       <c r="N29" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="R29" s="7" t="inlineStr">
         <is>
@@ -2513,16 +2519,16 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="30">
       <c r="C30" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>118</v>
+        <v>214</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>41</v>
@@ -2537,7 +2543,7 @@
         <v>5</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R30" s="7" t="inlineStr">
         <is>
@@ -2547,16 +2553,22 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="31">
       <c r="C31" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>164</v>
+        <v>220</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>41</v>
@@ -2571,10 +2583,10 @@
         <v>5</v>
       </c>
       <c r="N31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="P31" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="R31" s="7" t="inlineStr">
         <is>
@@ -2584,22 +2596,22 @@
     </row>
     <row spans="1:18" outlineLevel="0" r="32">
       <c r="C32" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>41</v>
@@ -2617,10 +2629,10 @@
         <v>62</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="R32" s="7" t="inlineStr">
         <is>
@@ -2630,22 +2642,16 @@
     </row>
     <row spans="2:18" outlineLevel="0" r="33">
       <c r="C33" s="3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>41</v>
@@ -2663,10 +2669,10 @@
         <v>62</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="R33" s="7" t="inlineStr">
         <is>
@@ -2676,23 +2682,26 @@
     </row>
     <row spans="2:18" outlineLevel="0" r="35">
       <c r="B35" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row spans="2:18" outlineLevel="0" r="36">
       <c r="B36" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D36" s="2" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row spans="2:18" outlineLevel="0" r="37">
       <c r="B37" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>6</v>
@@ -2700,10 +2709,16 @@
     </row>
     <row spans="2:18" outlineLevel="0" r="38">
       <c r="B38" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row spans="2:18" outlineLevel="0" r="40">
+      <c r="C40" s="4"/>
+      <c r="D40" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plant RANDOM function in the xlsx file not so much effect from it anyway.
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -7,12 +7,12 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="2" r:id="rId1" name="DataSet"/>
+    <sheet name="DataSet" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -100,12 +100,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>vankatabe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These two cells have functions inserted in an attempt to generate unique username and email every time a cell changes</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="222">
   <si>
     <t>Key</t>
   </si>
@@ -777,7 +801,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,8 +841,21 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,6 +874,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -850,7 +893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -863,6 +906,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,14 +1232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J3" sqref="I3:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23" style="2" customWidth="1"/>
@@ -1216,7 +1260,7 @@
     <col min="18" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:18" outlineLevel="0" r="1">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1272,7 +1316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row spans="1:18" outlineLevel="0" r="2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1341,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row spans="1:18" outlineLevel="0" r="3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1322,11 +1366,13 @@
       <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>40</v>
+      <c r="I3" s="10" t="str">
+        <f ca="1">CONCATENATE(J3, "@test.com")</f>
+        <v>randomuser23@test.com</v>
+      </c>
+      <c r="J3" s="10" t="str">
+        <f ca="1">CONCATENATE("randomuser",RANDBETWEEN(1,200))</f>
+        <v>randomuser23</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>5</v>
@@ -1342,13 +1388,11 @@
         <v>35</v>
       </c>
       <c r="Q3" s="4"/>
-      <c r="R3" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="4">
+      <c r="R3" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
@@ -1385,13 +1429,11 @@
       <c r="P4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="5">
+      <c r="R4" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
@@ -1428,13 +1470,11 @@
       <c r="P5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="R5" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="6">
+      <c r="R5" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -1477,13 +1517,11 @@
       <c r="Q6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="R6" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="7">
+      <c r="R6" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -1520,13 +1558,11 @@
       <c r="P7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="R7" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="8">
+      <c r="R7" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -1571,13 +1607,11 @@
         <v>35</v>
       </c>
       <c r="Q8" s="4"/>
-      <c r="R8" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="9">
+      <c r="R8" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
@@ -1616,13 +1650,11 @@
         <v>84</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="10">
+      <c r="R9" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
@@ -1663,13 +1695,11 @@
         <v>179</v>
       </c>
       <c r="Q10" s="3"/>
-      <c r="R10" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="11">
+      <c r="R10" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
@@ -1708,13 +1738,11 @@
         <v>74</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="12">
+      <c r="R11" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
@@ -1749,13 +1777,11 @@
         <v>184</v>
       </c>
       <c r="Q12" s="3"/>
-      <c r="R12" s="8" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="13">
+      <c r="R12" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1803,13 +1829,11 @@
         <v>64</v>
       </c>
       <c r="Q13" s="4"/>
-      <c r="R13" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="14">
+      <c r="R13" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -1853,13 +1877,11 @@
         <v>185</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="15">
+      <c r="R14" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -1901,13 +1923,11 @@
         <v>172</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="16">
+      <c r="R15" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
@@ -1951,13 +1971,11 @@
         <v>175</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="17">
+      <c r="R16" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>201</v>
       </c>
@@ -2005,13 +2023,11 @@
         <v>205</v>
       </c>
       <c r="Q17" s="4"/>
-      <c r="R17" s="7" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="18">
+      <c r="R17" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
@@ -2057,13 +2073,11 @@
         <v>54</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="19">
+      <c r="R18" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>65</v>
       </c>
@@ -2111,13 +2125,11 @@
         <v>72</v>
       </c>
       <c r="Q19" s="4"/>
-      <c r="R19" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="20">
+      <c r="R19" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
@@ -2159,13 +2171,11 @@
         <v>200</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="7" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="21">
+      <c r="R20" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>89</v>
       </c>
@@ -2213,13 +2223,11 @@
         <v>96</v>
       </c>
       <c r="Q21" s="4"/>
-      <c r="R21" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="22">
+      <c r="R21" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -2257,13 +2265,11 @@
         <v>30</v>
       </c>
       <c r="Q22" s="4"/>
-      <c r="R22" s="7" t="inlineStr">
-        <is>
-          <t>Inconclusive</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="23">
+      <c r="R22" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>132</v>
       </c>
@@ -2293,13 +2299,11 @@
         <v>159</v>
       </c>
       <c r="Q23" s="3"/>
-      <c r="R23" s="8" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="24">
+      <c r="R23" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
@@ -2322,13 +2326,11 @@
       <c r="P24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="R24" s="7" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="25">
+      <c r="R24" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
@@ -2351,13 +2353,11 @@
       <c r="P25" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="R25" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="26">
+      <c r="R25" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C26" s="3" t="s">
         <v>137</v>
       </c>
@@ -2394,13 +2394,11 @@
       <c r="Q26" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="R26" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="27">
+      <c r="R26" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>138</v>
       </c>
@@ -2431,13 +2429,11 @@
       <c r="P27" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="R27" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="28">
+      <c r="R27" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C28" s="3" t="s">
         <v>139</v>
       </c>
@@ -2471,13 +2467,11 @@
       <c r="P28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="R28" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="29">
+      <c r="R28" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C29" s="3" t="s">
         <v>140</v>
       </c>
@@ -2511,13 +2505,11 @@
       <c r="P29" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="R29" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="30">
+      <c r="R29" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C30" s="3" t="s">
         <v>141</v>
       </c>
@@ -2545,13 +2537,11 @@
       <c r="P30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R30" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="31">
+      <c r="R30" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C31" s="3" t="s">
         <v>142</v>
       </c>
@@ -2588,13 +2578,11 @@
       <c r="P31" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R31" s="7" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:18" outlineLevel="0" r="32">
+      <c r="R31" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C32" s="3" t="s">
         <v>186</v>
       </c>
@@ -2634,13 +2622,11 @@
       <c r="P32" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="R32" s="7" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="2:18" outlineLevel="0" r="33">
+      <c r="R32" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C33" s="3" t="s">
         <v>191</v>
       </c>
@@ -2674,13 +2660,11 @@
       <c r="P33" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="R33" s="7" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row spans="2:18" outlineLevel="0" r="35">
+      <c r="R33" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>145</v>
       </c>
@@ -2688,7 +2672,7 @@
         <v>144</v>
       </c>
     </row>
-    <row spans="2:18" outlineLevel="0" r="36">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>146</v>
       </c>
@@ -2699,7 +2683,7 @@
         <v>210</v>
       </c>
     </row>
-    <row spans="2:18" outlineLevel="0" r="37">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>147</v>
       </c>
@@ -2707,7 +2691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row spans="2:18" outlineLevel="0" r="38">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>148</v>
       </c>
@@ -2715,7 +2699,7 @@
         <v>42</v>
       </c>
     </row>
-    <row spans="2:18" outlineLevel="0" r="40">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C40" s="4"/>
       <c r="D40" s="2" t="s">
         <v>219</v>

</xml_diff>

<commit_message>
Minor improvements mainly in Documentation
</commit_message>
<xml_diff>
--- a/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -431,12 +431,6 @@
     <t>http://localhost:60639/Account/Login</t>
   </si>
   <si>
-    <t>Navigate to Register page</t>
-  </si>
-  <si>
-    <t>Navigate to Log in page</t>
-  </si>
-  <si>
     <t>http://localhost:60639/Account/Register</t>
   </si>
   <si>
@@ -602,9 +596,6 @@
     <t>Login_WithoutPassword_LoginUnsuccessful</t>
   </si>
   <si>
-    <t>Navigate to Home page through Logo link</t>
-  </si>
-  <si>
     <t>Account_ClickOnChangePassword_ChangePasswordPageLoaded</t>
   </si>
   <si>
@@ -707,9 +698,6 @@
     <t>10.11</t>
   </si>
   <si>
-    <t xml:space="preserve">View article Author </t>
-  </si>
-  <si>
     <t>Create_NavigateToArticle_ArticleAuthorExists</t>
   </si>
   <si>
@@ -770,31 +758,43 @@
     <t>Change password link</t>
   </si>
   <si>
-    <t>Log in and comment created Article</t>
-  </si>
-  <si>
-    <t>Log In and Select Article to Edit</t>
-  </si>
-  <si>
-    <t>Log In and Select Article to Delete</t>
-  </si>
-  <si>
-    <t>Log In and Read an Article</t>
-  </si>
-  <si>
-    <t>Navigate to Create Article and click Cancel</t>
-  </si>
-  <si>
-    <t>Log In and Enter Account Management</t>
-  </si>
-  <si>
     <t>= positive tests - regression/smoke</t>
   </si>
   <si>
-    <t>Log In and navigate to Password change Page</t>
-  </si>
-  <si>
     <t>Login_BlankEmail_Login_Unsuccessful</t>
+  </si>
+  <si>
+    <t>Visitor Navigate to Login page</t>
+  </si>
+  <si>
+    <t>Visitor Navigate to Register page</t>
+  </si>
+  <si>
+    <t>Visitor Navigate to Home page through Logo link</t>
+  </si>
+  <si>
+    <t>User Login and Enter Account Management</t>
+  </si>
+  <si>
+    <t>User Navigate to Create Article and click Cancel</t>
+  </si>
+  <si>
+    <t>User Login and Read an Article</t>
+  </si>
+  <si>
+    <t>User Login and Select Article to Delete</t>
+  </si>
+  <si>
+    <t>User Login and Select Article to Edit</t>
+  </si>
+  <si>
+    <t>User Login and navigate to Password change Page</t>
+  </si>
+  <si>
+    <t>User Login and Comment created Article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visitor View article Author </t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J3" sqref="I3:J3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1368,11 +1368,11 @@
       </c>
       <c r="I3" s="10" t="str">
         <f ca="1">CONCATENATE(J3, "@test.com")</f>
-        <v>randomuser23@test.com</v>
+        <v>randomuser134@test.com</v>
       </c>
       <c r="J3" s="10" t="str">
         <f ca="1">CONCATENATE("randomuser",RANDBETWEEN(1,200))</f>
-        <v>randomuser23</v>
+        <v>randomuser134</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>5</v>
@@ -1396,19 +1396,19 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>75</v>
@@ -1437,19 +1437,19 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>76</v>
@@ -1478,19 +1478,19 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>80</v>
@@ -1525,19 +1525,19 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>86</v>
@@ -1615,22 +1615,22 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>4</v>
@@ -1658,22 +1658,22 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>41</v>
@@ -1688,11 +1688,11 @@
         <v>5</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="8" t="s">
@@ -1703,22 +1703,22 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="2" t="s">
@@ -1746,35 +1746,35 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I12" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="I12" t="s">
-        <v>182</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="8" t="s">
@@ -1837,22 +1837,22 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>41</v>
@@ -1870,11 +1870,11 @@
         <v>62</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="7" t="s">
@@ -1885,22 +1885,22 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>69</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>41</v>
@@ -1916,11 +1916,11 @@
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="7" t="s">
@@ -1931,22 +1931,22 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>41</v>
@@ -1964,11 +1964,11 @@
         <v>62</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="7" t="s">
@@ -1977,28 +1977,28 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>41</v>
@@ -2016,15 +2016,15 @@
         <v>62</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
@@ -2133,22 +2133,22 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>41</v>
@@ -2164,15 +2164,15 @@
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
@@ -2271,24 +2271,24 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I23" s="9"/>
       <c r="N23" t="s">
@@ -2296,62 +2296,62 @@
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>100</v>
+        <v>212</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>88</v>
@@ -2359,16 +2359,16 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C26" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>41</v>
@@ -2383,16 +2383,16 @@
         <v>5</v>
       </c>
       <c r="N26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="R26" s="7" t="s">
         <v>88</v>
@@ -2400,16 +2400,16 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>41</v>
@@ -2424,10 +2424,10 @@
         <v>5</v>
       </c>
       <c r="N27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>88</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C28" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>6</v>
@@ -2444,7 +2444,7 @@
         <v>216</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>41</v>
@@ -2473,16 +2473,16 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C29" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>41</v>
@@ -2500,10 +2500,10 @@
         <v>62</v>
       </c>
       <c r="N29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>88</v>
@@ -2511,16 +2511,16 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>41</v>
@@ -2535,7 +2535,7 @@
         <v>5</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R30" s="7" t="s">
         <v>88</v>
@@ -2543,22 +2543,22 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C31" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>41</v>
@@ -2573,10 +2573,10 @@
         <v>5</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>88</v>
@@ -2584,22 +2584,22 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C32" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>41</v>
@@ -2617,27 +2617,27 @@
         <v>62</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="R32" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C33" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>41</v>
@@ -2655,37 +2655,37 @@
         <v>62</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="R33" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>6</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>42</v>
@@ -2702,7 +2702,7 @@
     <row r="40" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C40" s="4"/>
       <c r="D40" s="2" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>